<commit_message>
Export final gerbers for MB
</commit_message>
<xml_diff>
--- a/morro-bay/PCB_Morro_Bay/Bom_Digi.xlsx
+++ b/morro-bay/PCB_Morro_Bay/Bom_Digi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper Rubin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasper Rubin\Desktop\Projects\Hyperloop\testing-hardware\morro-bay\PCB_Morro_Bay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35AB5F36-FCDB-4ED9-9E73-603A4699C762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755C49E4-55A9-4690-AD64-85BE8FE6F396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -744,10 +744,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1065,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2236,7 +2239,7 @@
       </c>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37">
+      <c r="A37" s="3">
         <v>5015</v>
       </c>
       <c r="B37" t="s">

</xml_diff>